<commit_message>
WS Update: Relationship, control panel, datasets
</commit_message>
<xml_diff>
--- a/ResultDataNew.xlsx
+++ b/ResultDataNew.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26606"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11208"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huyennguyen/Documents/GitHub/WordStreamV2/WordStream/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huyennguyen/Huyen/GitHub/WordStream/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A04CEDC5-FDC2-3A4E-8D5A-1C70EDB366D2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17220" yWindow="460" windowWidth="33820" windowHeight="27020" tabRatio="500"/>
+    <workbookView xWindow="2860" yWindow="3060" windowWidth="32520" windowHeight="27020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="24">
   <si>
     <t>Flow</t>
   </si>
@@ -68,9 +69,6 @@
     <t>IMDB</t>
   </si>
   <si>
-    <t>Popcha</t>
-  </si>
-  <si>
     <t>Cards_PC</t>
   </si>
   <si>
@@ -97,12 +95,15 @@
   <si>
     <t>Avg Freq</t>
   </si>
+  <si>
+    <t>tfidf</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -110,13 +111,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="9">
@@ -208,10 +233,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -255,20 +282,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -277,12 +333,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -321,7 +380,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -358,10 +416,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0572509186246902"/>
-          <c:y val="0.125604562850216"/>
-          <c:w val="0.94274908137531"/>
-          <c:h val="0.726459028126814"/>
+          <c:x val="5.72509186246902E-2"/>
+          <c:y val="0.12560456285021601"/>
+          <c:w val="0.94274908137530999"/>
+          <c:h val="0.72645902812681395"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -373,7 +431,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$O$22</c:f>
+              <c:f>Sheet1!$S$22</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -394,9 +452,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$C$22:$M$22</c:f>
+              <c:f>Sheet1!$D$22:$P$22</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>WikiNews</c:v>
                 </c:pt>
@@ -409,25 +467,25 @@
                 <c:pt idx="3">
                   <c:v>EmptyWheel</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>Esquire</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>FactCheck</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>VIS_paper</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>IMDB</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>PopCha</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>Cards_PC</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>Cards_Fries</c:v>
                 </c:pt>
               </c:strCache>
@@ -435,53 +493,25 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$23:$M$23</c:f>
+              <c:f>Sheet1!$D$23:$P$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>0.75</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.74</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.72</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.76</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.71</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.65</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.69</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.59</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.49</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.62</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.73</c:v>
-                </c:pt>
+                <c:ptCount val="13"/>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8F46-B644-B5F6-7C7567C49010}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$P$22</c:f>
+              <c:f>Sheet1!$T$22</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -502,9 +532,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$C$22:$M$22</c:f>
+              <c:f>Sheet1!$D$22:$P$22</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>WikiNews</c:v>
                 </c:pt>
@@ -517,25 +547,25 @@
                 <c:pt idx="3">
                   <c:v>EmptyWheel</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>Esquire</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>FactCheck</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>VIS_paper</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>IMDB</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>PopCha</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>Cards_PC</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>Cards_Fries</c:v>
                 </c:pt>
               </c:strCache>
@@ -543,53 +573,25 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$24:$M$24</c:f>
+              <c:f>Sheet1!$D$24:$P$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.79</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.77</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.76</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.76</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.65</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.55</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.68</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.77</c:v>
-                </c:pt>
+                <c:ptCount val="13"/>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8F46-B644-B5F6-7C7567C49010}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$Q$22</c:f>
+              <c:f>Sheet1!$U$22</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -610,9 +612,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$C$22:$M$22</c:f>
+              <c:f>Sheet1!$D$22:$P$22</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>WikiNews</c:v>
                 </c:pt>
@@ -625,25 +627,25 @@
                 <c:pt idx="3">
                   <c:v>EmptyWheel</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>Esquire</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>FactCheck</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>VIS_paper</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>IMDB</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>PopCha</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>Cards_PC</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>Cards_Fries</c:v>
                 </c:pt>
               </c:strCache>
@@ -651,53 +653,25 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$25:$M$25</c:f>
+              <c:f>Sheet1!$D$25:$P$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>0.76</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.76</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.74</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.79</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.73</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.67</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.71</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.61</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.45</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.64</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.75</c:v>
-                </c:pt>
+                <c:ptCount val="13"/>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-8F46-B644-B5F6-7C7567C49010}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$R$22</c:f>
+              <c:f>Sheet1!$V$22</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -718,9 +692,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$C$22:$M$22</c:f>
+              <c:f>Sheet1!$D$22:$P$22</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>WikiNews</c:v>
                 </c:pt>
@@ -733,25 +707,25 @@
                 <c:pt idx="3">
                   <c:v>EmptyWheel</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>Esquire</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>FactCheck</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>VIS_paper</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>IMDB</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>PopCha</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>Cards_PC</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>Cards_Fries</c:v>
                 </c:pt>
               </c:strCache>
@@ -759,46 +733,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$26:$M$26</c:f>
+              <c:f>Sheet1!$D$26:$P$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>0.88</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.88</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.86</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.91</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.85</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.78</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.82</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.74</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.53</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.73</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.84</c:v>
-                </c:pt>
+                <c:ptCount val="13"/>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-8F46-B644-B5F6-7C7567C49010}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -935,9 +881,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.205398037423803"/>
-          <c:y val="0.928599457104437"/>
-          <c:w val="0.589203811713928"/>
-          <c:h val="0.0714006466854962"/>
+          <c:y val="0.92859945710443703"/>
+          <c:w val="0.58920381171392799"/>
+          <c:h val="7.14006466854962E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1007,7 +953,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1046,7 +992,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1088,7 +1033,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$O$22</c:f>
+              <c:f>Sheet1!$S$22</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1109,9 +1054,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$C$22:$M$22</c:f>
+              <c:f>Sheet1!$D$22:$P$22</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>WikiNews</c:v>
                 </c:pt>
@@ -1124,25 +1069,25 @@
                 <c:pt idx="3">
                   <c:v>EmptyWheel</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>Esquire</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>FactCheck</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>VIS_paper</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>IMDB</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>PopCha</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>Cards_PC</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>Cards_Fries</c:v>
                 </c:pt>
               </c:strCache>
@@ -1150,53 +1095,25 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$29:$M$29</c:f>
+              <c:f>Sheet1!$D$29:$P$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>0.65</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.64</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.7</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.73</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.63</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.61</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.65</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.54</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.77</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.84</c:v>
-                </c:pt>
+                <c:ptCount val="13"/>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-44A1-0841-9B1A-F4E099903FF8}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$P$22</c:f>
+              <c:f>Sheet1!$T$22</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1217,9 +1134,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$C$22:$M$22</c:f>
+              <c:f>Sheet1!$D$22:$P$22</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>WikiNews</c:v>
                 </c:pt>
@@ -1232,25 +1149,25 @@
                 <c:pt idx="3">
                   <c:v>EmptyWheel</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>Esquire</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>FactCheck</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>VIS_paper</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>IMDB</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>PopCha</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>Cards_PC</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>Cards_Fries</c:v>
                 </c:pt>
               </c:strCache>
@@ -1258,53 +1175,25 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$30:$M$30</c:f>
+              <c:f>Sheet1!$D$30:$P$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>0.68</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.67</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.73</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.75</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.66</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.63</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.71</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.59</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.56</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.81</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.86</c:v>
-                </c:pt>
+                <c:ptCount val="13"/>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-44A1-0841-9B1A-F4E099903FF8}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$Q$22</c:f>
+              <c:f>Sheet1!$U$22</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1325,9 +1214,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$C$22:$M$22</c:f>
+              <c:f>Sheet1!$D$22:$P$22</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>WikiNews</c:v>
                 </c:pt>
@@ -1340,25 +1229,25 @@
                 <c:pt idx="3">
                   <c:v>EmptyWheel</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>Esquire</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>FactCheck</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>VIS_paper</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>IMDB</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>PopCha</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>Cards_PC</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>Cards_Fries</c:v>
                 </c:pt>
               </c:strCache>
@@ -1366,53 +1255,25 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$31:$M$31</c:f>
+              <c:f>Sheet1!$D$31:$P$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>0.66</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.65</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.71</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.75</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.65</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.62</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.67</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.55</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.48</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.78</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.85</c:v>
-                </c:pt>
+                <c:ptCount val="13"/>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-44A1-0841-9B1A-F4E099903FF8}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$R$22</c:f>
+              <c:f>Sheet1!$V$22</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1433,9 +1294,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$C$22:$M$22</c:f>
+              <c:f>Sheet1!$D$22:$P$22</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>WikiNews</c:v>
                 </c:pt>
@@ -1448,25 +1309,25 @@
                 <c:pt idx="3">
                   <c:v>EmptyWheel</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>Esquire</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>FactCheck</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>VIS_paper</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>IMDB</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>PopCha</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>Cards_PC</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>Cards_Fries</c:v>
                 </c:pt>
               </c:strCache>
@@ -1474,46 +1335,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$32:$M$32</c:f>
+              <c:f>Sheet1!$D$32:$P$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>0.73</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.72</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.78</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.71</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.69</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.78</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.67</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.56</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.84</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.9</c:v>
-                </c:pt>
+                <c:ptCount val="13"/>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-44A1-0841-9B1A-F4E099903FF8}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1649,10 +1482,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.204096472712875"/>
-          <c:y val="0.914690834815398"/>
-          <c:w val="0.59180705457425"/>
-          <c:h val="0.0720928532997621"/>
+          <c:x val="0.20409647271287501"/>
+          <c:y val="0.91469083481539804"/>
+          <c:w val="0.59180705457424998"/>
+          <c:h val="7.2092853299762102E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1722,7 +1555,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1761,7 +1594,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1803,7 +1635,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$O$22</c:f>
+              <c:f>Sheet1!$S$22</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1824,9 +1656,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$C$22:$M$22</c:f>
+              <c:f>Sheet1!$D$22:$P$22</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>WikiNews</c:v>
                 </c:pt>
@@ -1839,25 +1671,25 @@
                 <c:pt idx="3">
                   <c:v>EmptyWheel</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>Esquire</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>FactCheck</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>VIS_paper</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>IMDB</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>PopCha</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>Cards_PC</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>Cards_Fries</c:v>
                 </c:pt>
               </c:strCache>
@@ -1865,53 +1697,25 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$35:$M$35</c:f>
+              <c:f>Sheet1!$D$35:$P$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>0.113</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.062</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.064</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.109</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.076</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.075</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.252</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.191</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.051</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.06</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.081</c:v>
-                </c:pt>
+                <c:ptCount val="13"/>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7479-284C-B568-D6224E1293A4}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$P$22</c:f>
+              <c:f>Sheet1!$T$22</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1932,9 +1736,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$C$22:$M$22</c:f>
+              <c:f>Sheet1!$D$22:$P$22</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>WikiNews</c:v>
                 </c:pt>
@@ -1947,25 +1751,25 @@
                 <c:pt idx="3">
                   <c:v>EmptyWheel</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>Esquire</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>FactCheck</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>VIS_paper</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>IMDB</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>PopCha</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>Cards_PC</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>Cards_Fries</c:v>
                 </c:pt>
               </c:strCache>
@@ -1973,53 +1777,25 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$36:$M$36</c:f>
+              <c:f>Sheet1!$D$36:$P$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>0.113</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.061</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.064</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.107</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.076</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.075</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.25</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.191</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.051</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.061</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.08</c:v>
-                </c:pt>
+                <c:ptCount val="13"/>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7479-284C-B568-D6224E1293A4}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$Q$22</c:f>
+              <c:f>Sheet1!$U$22</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2040,9 +1816,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$C$22:$M$22</c:f>
+              <c:f>Sheet1!$D$22:$P$22</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>WikiNews</c:v>
                 </c:pt>
@@ -2055,25 +1831,25 @@
                 <c:pt idx="3">
                   <c:v>EmptyWheel</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>Esquire</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>FactCheck</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>VIS_paper</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>IMDB</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>PopCha</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>Cards_PC</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>Cards_Fries</c:v>
                 </c:pt>
               </c:strCache>
@@ -2081,53 +1857,25 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$37:$M$37</c:f>
+              <c:f>Sheet1!$D$37:$P$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>0.111</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.061</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.064</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.107</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.075</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.075</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.251</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.19</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.05</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.058</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.08</c:v>
-                </c:pt>
+                <c:ptCount val="13"/>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-7479-284C-B568-D6224E1293A4}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$R$22</c:f>
+              <c:f>Sheet1!$V$22</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2148,9 +1896,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$C$22:$M$22</c:f>
+              <c:f>Sheet1!$D$22:$P$22</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>WikiNews</c:v>
                 </c:pt>
@@ -2163,25 +1911,25 @@
                 <c:pt idx="3">
                   <c:v>EmptyWheel</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>Esquire</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>FactCheck</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>VIS_paper</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>IMDB</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>PopCha</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>Cards_PC</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>Cards_Fries</c:v>
                 </c:pt>
               </c:strCache>
@@ -2189,46 +1937,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$38:$M$38</c:f>
+              <c:f>Sheet1!$D$38:$P$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>0.11</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.059</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.062</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.103</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.073</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.074</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.248</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.19</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.05</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.057</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.076</c:v>
-                </c:pt>
+                <c:ptCount val="13"/>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-7479-284C-B568-D6224E1293A4}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2360,7 +2080,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4060,20 +3779,26 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>161899</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>242366</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>530296</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>135726</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>106641</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>193890</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>87249</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4090,20 +3815,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>132815</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>242365</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>74647</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>145419</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>465344</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>193698</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>407176</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>96751</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4120,20 +3851,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>695108</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>271450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
+      <xdr:col>34</xdr:col>
       <xdr:colOff>300535</xdr:colOff>
       <xdr:row>52</xdr:row>
       <xdr:rowOff>184198</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4413,117 +4150,125 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:Z38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A3:AG38"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="J22" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="131" workbookViewId="0">
-      <selection activeCell="N35" sqref="N35"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="C1" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="131" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="12" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.1640625" style="1" customWidth="1"/>
-    <col min="6" max="14" width="12" style="1" customWidth="1"/>
-    <col min="15" max="15" width="25.83203125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12" style="1" customWidth="1"/>
-    <col min="17" max="17" width="25.1640625" style="1" customWidth="1"/>
-    <col min="18" max="29" width="12" style="1" customWidth="1"/>
-    <col min="30" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="2" width="12" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.1640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12" style="1" customWidth="1"/>
+    <col min="8" max="8" width="24.5" style="1" customWidth="1"/>
+    <col min="9" max="12" width="12" style="1" customWidth="1"/>
+    <col min="13" max="13" width="23.6640625" style="1" customWidth="1"/>
+    <col min="14" max="17" width="12" style="1" customWidth="1"/>
+    <col min="18" max="18" width="23" style="26" customWidth="1"/>
+    <col min="19" max="19" width="15.6640625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="12" style="1" customWidth="1"/>
+    <col min="21" max="21" width="25.1640625" style="1" customWidth="1"/>
+    <col min="22" max="22" width="12" style="1" customWidth="1"/>
+    <col min="23" max="23" width="22" style="1" customWidth="1"/>
+    <col min="24" max="27" width="12" style="1" customWidth="1"/>
+    <col min="28" max="28" width="19.1640625" style="1" customWidth="1"/>
+    <col min="29" max="36" width="12" style="1" customWidth="1"/>
+    <col min="37" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:26" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C3" s="15" t="s">
+    <row r="3" spans="1:33" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C3" s="17"/>
+      <c r="D3" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="15" t="s">
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="15" t="s">
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="15" t="s">
+      <c r="O3" s="19"/>
+      <c r="P3" s="19"/>
+      <c r="Q3" s="25"/>
+      <c r="R3" s="27"/>
+      <c r="S3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="P3" s="16"/>
-      <c r="Q3" s="16"/>
-      <c r="R3" s="17"/>
-      <c r="S3" s="15" t="s">
+      <c r="T3" s="22"/>
+      <c r="U3" s="22"/>
+      <c r="V3" s="23"/>
+      <c r="W3" s="24"/>
+      <c r="X3" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="T3" s="16"/>
-      <c r="U3" s="16"/>
-      <c r="V3" s="17"/>
-      <c r="W3" s="15" t="s">
+      <c r="Y3" s="19"/>
+      <c r="Z3" s="19"/>
+      <c r="AA3" s="25"/>
+      <c r="AB3" s="20"/>
+      <c r="AC3" s="20"/>
+      <c r="AD3" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="X3" s="16"/>
-      <c r="Y3" s="16"/>
-      <c r="Z3" s="17"/>
+      <c r="AE3" s="22"/>
+      <c r="AF3" s="22"/>
+      <c r="AG3" s="23"/>
     </row>
-    <row r="4" spans="1:26" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:33" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="E4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="F4" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="G4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="H4" s="14"/>
+      <c r="I4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="J4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="K4" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="L4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="M4" s="14"/>
+      <c r="N4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="L4" s="10" t="s">
+      <c r="O4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="M4" s="10" t="s">
+      <c r="P4" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="N4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="P4" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q4" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="R4" s="5" t="s">
+      <c r="Q4" s="5" t="s">
         <v>6</v>
       </c>
       <c r="S4" s="4" t="s">
@@ -4538,1234 +4283,1135 @@
       <c r="V4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="W4" s="4" t="s">
+      <c r="W4" s="14"/>
+      <c r="X4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="X4" s="10" t="s">
+      <c r="Y4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="Y4" s="10" t="s">
+      <c r="Z4" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="Z4" s="5" t="s">
+      <c r="AA4" s="5" t="s">
         <v>6</v>
       </c>
+      <c r="AB4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD4" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF4" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="5" spans="1:26" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:33" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.52</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.88</v>
+      </c>
+      <c r="E5" s="10">
+        <v>1.61</v>
+      </c>
+      <c r="F5" s="10">
+        <v>0.78</v>
+      </c>
+      <c r="G5" s="14">
+        <v>0.09</v>
+      </c>
+      <c r="H5" s="14">
+        <v>0.71</v>
+      </c>
+      <c r="I5" s="4">
+        <v>0.82</v>
+      </c>
+      <c r="J5" s="10">
+        <v>1.17</v>
+      </c>
+      <c r="K5" s="10">
+        <v>0.87</v>
+      </c>
+      <c r="L5" s="5">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="M5" s="14">
+        <v>0.71</v>
+      </c>
+      <c r="N5" s="4">
+        <v>0.83</v>
+      </c>
+      <c r="O5" s="10">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="P5" s="10">
+        <v>0.9</v>
+      </c>
+      <c r="Q5" s="5">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="R5" s="26">
+        <v>0.88</v>
+      </c>
+      <c r="S5" s="4">
+        <v>0.88</v>
+      </c>
+      <c r="T5" s="10">
         <v>1</v>
       </c>
-      <c r="B5" s="1">
+      <c r="U5" s="10">
+        <v>0.94</v>
+      </c>
+      <c r="V5" s="5">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="W5" s="14">
+        <v>0.73</v>
+      </c>
+      <c r="X5" s="4">
+        <v>0.83</v>
+      </c>
+      <c r="Y5" s="10">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="Z5" s="10">
+        <v>0.86</v>
+      </c>
+      <c r="AA5" s="5">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="AB5" s="14">
+        <v>0.65</v>
+      </c>
+      <c r="AC5" s="14">
+        <v>0.83</v>
+      </c>
+      <c r="AD5" s="4">
+        <v>1.3</v>
+      </c>
+      <c r="AE5" s="10">
+        <v>0.78</v>
+      </c>
+      <c r="AF5" s="10">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="AG5" s="5"/>
+    </row>
+    <row r="6" spans="1:33" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>0</v>
+      </c>
+      <c r="B6" s="1">
         <v>1</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C6" s="1">
+        <v>0.46</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.77</v>
+      </c>
+      <c r="E6" s="10">
+        <v>1.61</v>
+      </c>
+      <c r="F6" s="10">
+        <v>0.72</v>
+      </c>
+      <c r="G6" s="10">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="H6" s="14">
+        <v>0.65</v>
+      </c>
+      <c r="I6" s="4">
+        <v>0.73</v>
+      </c>
+      <c r="J6" s="10">
+        <v>1.17</v>
+      </c>
+      <c r="K6" s="10">
+        <v>0.81</v>
+      </c>
+      <c r="L6" s="5">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="M6" s="14">
+        <v>0.63</v>
+      </c>
+      <c r="N6" s="4">
+        <v>0.72</v>
+      </c>
+      <c r="O6" s="10">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="P6" s="10">
+        <v>0.84</v>
+      </c>
+      <c r="Q6" s="5">
+        <v>5.5E-2</v>
+      </c>
+      <c r="R6" s="26">
+        <v>0.79</v>
+      </c>
+      <c r="S6" s="4">
+        <v>0.77</v>
+      </c>
+      <c r="T6" s="10">
+        <v>1</v>
+      </c>
+      <c r="U6" s="10">
+        <v>0.88</v>
+      </c>
+      <c r="V6" s="5">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="W6" s="14">
+        <v>0.64</v>
+      </c>
+      <c r="X6" s="4">
+        <v>0.72</v>
+      </c>
+      <c r="Y6" s="10">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="Z6" s="10">
+        <v>0.79</v>
+      </c>
+      <c r="AA6" s="5">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="AB6" s="14">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="AC6" s="14">
+        <v>0.69</v>
+      </c>
+      <c r="AD6" s="4">
+        <v>1.3</v>
+      </c>
+      <c r="AE6" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="AF6" s="10">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="AG6" s="5"/>
+    </row>
+    <row r="7" spans="1:33" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>1</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.48</v>
+      </c>
+      <c r="D7" s="6">
+        <v>0.81</v>
+      </c>
+      <c r="E7" s="10">
+        <v>1.61</v>
+      </c>
+      <c r="F7" s="10">
+        <v>0.74</v>
+      </c>
+      <c r="G7" s="10">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="H7" s="14">
+        <v>0.66</v>
+      </c>
+      <c r="I7" s="4">
+        <v>0.76</v>
+      </c>
+      <c r="J7" s="10">
+        <v>1.17</v>
+      </c>
+      <c r="K7" s="10">
+        <v>0.83</v>
+      </c>
+      <c r="L7" s="5">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="M7" s="14">
+        <v>0.65</v>
+      </c>
+      <c r="N7" s="4">
+        <v>0.76</v>
+      </c>
+      <c r="O7" s="10">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="P7" s="10">
+        <v>0.85</v>
+      </c>
+      <c r="Q7" s="5">
+        <v>5.5E-2</v>
+      </c>
+      <c r="R7" s="26">
+        <v>0.81</v>
+      </c>
+      <c r="S7" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="T7" s="10">
+        <v>1</v>
+      </c>
+      <c r="U7" s="10">
+        <v>0.9</v>
+      </c>
+      <c r="V7" s="5">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="W7" s="14">
+        <v>0.67</v>
+      </c>
+      <c r="X7" s="4">
         <v>0.75</v>
       </c>
-      <c r="D5" s="10">
-        <v>1.71</v>
-      </c>
-      <c r="E5" s="10">
-        <v>0.65</v>
-      </c>
-      <c r="F5" s="10">
-        <v>0.113</v>
-      </c>
-      <c r="G5" s="4">
-        <v>0.74</v>
-      </c>
-      <c r="H5" s="10">
-        <v>1.75</v>
-      </c>
-      <c r="I5" s="10">
+      <c r="Y7" s="10">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="Z7" s="10">
+        <v>0.81</v>
+      </c>
+      <c r="AA7" s="5">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="AB7" s="14">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="AC7" s="14">
+        <v>0.73</v>
+      </c>
+      <c r="AD7" s="4">
+        <v>1.3</v>
+      </c>
+      <c r="AE7" s="10">
+        <v>0.72</v>
+      </c>
+      <c r="AF7" s="10">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="AG7" s="5"/>
+    </row>
+    <row r="8" spans="1:33" s="8" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="8">
+        <v>1</v>
+      </c>
+      <c r="B8" s="8">
+        <v>1</v>
+      </c>
+      <c r="C8" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="D8" s="7">
+        <v>0.75</v>
+      </c>
+      <c r="E8" s="8">
+        <v>1.61</v>
+      </c>
+      <c r="F8" s="8">
+        <v>0.71</v>
+      </c>
+      <c r="G8" s="9">
+        <v>9.4E-2</v>
+      </c>
+      <c r="H8" s="8">
         <v>0.64</v>
       </c>
-      <c r="J5" s="5">
-        <v>6.2E-2</v>
-      </c>
-      <c r="K5" s="4">
-        <v>0.72</v>
-      </c>
-      <c r="L5" s="10">
-        <v>1.56</v>
-      </c>
-      <c r="M5" s="10">
+      <c r="I8" s="7">
+        <v>0.71</v>
+      </c>
+      <c r="J8" s="8">
+        <v>1.17</v>
+      </c>
+      <c r="K8" s="8">
+        <v>0.81</v>
+      </c>
+      <c r="L8" s="9">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="M8" s="8">
+        <v>0.62</v>
+      </c>
+      <c r="N8" s="7">
         <v>0.7</v>
       </c>
-      <c r="N5" s="5">
-        <v>6.4000000000000001E-2</v>
-      </c>
-      <c r="O5" s="4">
-        <v>0.76</v>
-      </c>
-      <c r="P5" s="10">
-        <v>1.38</v>
-      </c>
-      <c r="Q5" s="10">
-        <v>0.73</v>
-      </c>
-      <c r="R5" s="5">
-        <v>0.109</v>
-      </c>
-      <c r="S5" s="4">
-        <v>0.71</v>
-      </c>
-      <c r="T5" s="10">
-        <v>1.57</v>
-      </c>
-      <c r="U5" s="10">
-        <v>0.63</v>
-      </c>
-      <c r="V5" s="5">
-        <v>7.5999999999999998E-2</v>
-      </c>
-      <c r="W5" s="4">
-        <v>0.65</v>
-      </c>
-      <c r="X5" s="10">
-        <v>1.54</v>
-      </c>
-      <c r="Y5" s="10">
-        <v>0.61</v>
-      </c>
-      <c r="Z5" s="5">
-        <v>7.4999999999999997E-2</v>
-      </c>
+      <c r="O8" s="8">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="P8" s="8">
+        <v>0.83</v>
+      </c>
+      <c r="Q8" s="9">
+        <v>5.5E-2</v>
+      </c>
+      <c r="R8" s="8">
+        <v>0.77</v>
+      </c>
+      <c r="S8" s="7">
+        <v>0.75</v>
+      </c>
+      <c r="T8" s="8">
+        <v>1</v>
+      </c>
+      <c r="U8" s="8">
+        <v>0.87</v>
+      </c>
+      <c r="V8" s="9">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="W8" s="8">
+        <v>0.62</v>
+      </c>
+      <c r="X8" s="7">
+        <v>0.69</v>
+      </c>
+      <c r="Y8" s="8">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="Z8" s="8">
+        <v>0.77</v>
+      </c>
+      <c r="AA8" s="9">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="AB8" s="8">
+        <v>0.54</v>
+      </c>
+      <c r="AC8" s="8">
+        <v>0.66</v>
+      </c>
+      <c r="AD8" s="7">
+        <v>1.3</v>
+      </c>
+      <c r="AE8" s="8">
+        <v>0.68</v>
+      </c>
+      <c r="AF8" s="8">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="AG8" s="9"/>
     </row>
-    <row r="6" spans="1:26" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>1</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0</v>
-      </c>
-      <c r="C6" s="4">
-        <v>0.8</v>
-      </c>
-      <c r="D6" s="10">
-        <v>1.71</v>
-      </c>
-      <c r="E6" s="10">
-        <v>0.68</v>
-      </c>
-      <c r="F6" s="10">
-        <v>0.113</v>
-      </c>
-      <c r="G6" s="4">
-        <v>0.79</v>
-      </c>
-      <c r="H6" s="10">
-        <v>1.75</v>
-      </c>
-      <c r="I6" s="10">
-        <v>0.67</v>
-      </c>
-      <c r="J6" s="5">
-        <v>6.0999999999999999E-2</v>
-      </c>
-      <c r="K6" s="4">
-        <v>0.77</v>
-      </c>
-      <c r="L6" s="10">
-        <v>1.56</v>
-      </c>
-      <c r="M6" s="10">
-        <v>0.73</v>
-      </c>
-      <c r="N6" s="5">
-        <v>6.4000000000000001E-2</v>
-      </c>
-      <c r="O6" s="4">
-        <v>0.8</v>
-      </c>
-      <c r="P6" s="10">
-        <v>1.38</v>
-      </c>
-      <c r="Q6" s="10">
-        <v>0.75</v>
-      </c>
-      <c r="R6" s="5">
-        <v>0.107</v>
-      </c>
-      <c r="S6" s="4">
-        <v>0.76</v>
-      </c>
-      <c r="T6" s="10">
-        <v>1.57</v>
-      </c>
-      <c r="U6" s="10">
-        <v>0.66</v>
-      </c>
-      <c r="V6" s="5">
-        <v>7.5999999999999998E-2</v>
-      </c>
-      <c r="W6" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="X6" s="10">
-        <v>1.54</v>
-      </c>
-      <c r="Y6" s="10">
-        <v>0.63</v>
-      </c>
-      <c r="Z6" s="5">
-        <v>7.4999999999999997E-2</v>
-      </c>
+    <row r="9" spans="1:33" s="15" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:33" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C11" s="17"/>
+      <c r="D11" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="24"/>
+      <c r="N11" s="18"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="25"/>
+      <c r="R11" s="27"/>
+      <c r="S11" s="21"/>
+      <c r="T11" s="22"/>
+      <c r="U11" s="22"/>
+      <c r="V11" s="23"/>
+      <c r="W11" s="24"/>
+      <c r="X11" s="18"/>
+      <c r="Y11" s="19"/>
+      <c r="Z11" s="19"/>
+      <c r="AA11" s="25"/>
+      <c r="AB11"/>
+      <c r="AC11" s="14"/>
+      <c r="AD11" s="16"/>
+      <c r="AE11" s="16"/>
+      <c r="AF11" s="16"/>
+      <c r="AG11" s="16"/>
     </row>
-    <row r="7" spans="1:26" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
-        <v>0</v>
-      </c>
-      <c r="B7" s="2">
-        <v>1</v>
-      </c>
-      <c r="C7" s="6">
-        <v>0.76</v>
-      </c>
-      <c r="D7" s="10">
-        <v>1.71</v>
-      </c>
-      <c r="E7" s="10">
-        <v>0.66</v>
-      </c>
-      <c r="F7" s="10">
-        <v>0.111</v>
-      </c>
-      <c r="G7" s="4">
-        <v>0.76</v>
-      </c>
-      <c r="H7" s="10">
-        <v>1.75</v>
-      </c>
-      <c r="I7" s="10">
-        <v>0.65</v>
-      </c>
-      <c r="J7" s="5">
-        <v>6.0999999999999999E-2</v>
-      </c>
-      <c r="K7" s="4">
-        <v>0.74</v>
-      </c>
-      <c r="L7" s="10">
-        <v>1.56</v>
-      </c>
-      <c r="M7" s="10">
-        <v>0.71</v>
-      </c>
-      <c r="N7" s="5">
-        <v>6.4000000000000001E-2</v>
-      </c>
-      <c r="O7" s="4">
-        <v>0.79</v>
-      </c>
-      <c r="P7" s="10">
-        <v>1.38</v>
-      </c>
-      <c r="Q7" s="10">
-        <v>0.75</v>
-      </c>
-      <c r="R7" s="5">
-        <v>0.107</v>
-      </c>
-      <c r="S7" s="4">
-        <v>0.73</v>
-      </c>
-      <c r="T7" s="10">
-        <v>1.57</v>
-      </c>
-      <c r="U7" s="10">
-        <v>0.65</v>
-      </c>
-      <c r="V7" s="5">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="W7" s="4">
-        <v>0.67</v>
-      </c>
-      <c r="X7" s="10">
-        <v>1.54</v>
-      </c>
-      <c r="Y7" s="10">
-        <v>0.62</v>
-      </c>
-      <c r="Z7" s="5">
-        <v>7.4999999999999997E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" s="8" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="8">
-        <v>0</v>
-      </c>
-      <c r="B8" s="8">
-        <v>0</v>
-      </c>
-      <c r="C8" s="7">
-        <v>0.88</v>
-      </c>
-      <c r="D8" s="8">
-        <v>1.71</v>
-      </c>
-      <c r="E8" s="8">
-        <v>0.73</v>
-      </c>
-      <c r="F8" s="9">
-        <v>0.11</v>
-      </c>
-      <c r="G8" s="7">
-        <v>0.88</v>
-      </c>
-      <c r="H8" s="8">
-        <v>1.75</v>
-      </c>
-      <c r="I8" s="8">
-        <v>0.72</v>
-      </c>
-      <c r="J8" s="9">
-        <v>5.8999999999999997E-2</v>
-      </c>
-      <c r="K8" s="7">
-        <v>0.86</v>
-      </c>
-      <c r="L8" s="8">
-        <v>1.56</v>
-      </c>
-      <c r="M8" s="8">
-        <v>0.78</v>
-      </c>
-      <c r="N8" s="9">
-        <v>6.2E-2</v>
-      </c>
-      <c r="O8" s="7">
-        <v>0.91</v>
-      </c>
-      <c r="P8" s="8">
-        <v>1.38</v>
-      </c>
-      <c r="Q8" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="R8" s="9">
-        <v>0.10299999999999999</v>
-      </c>
-      <c r="S8" s="7">
-        <v>0.85</v>
-      </c>
-      <c r="T8" s="8">
-        <v>1.57</v>
-      </c>
-      <c r="U8" s="8">
-        <v>0.71</v>
-      </c>
-      <c r="V8" s="9">
-        <v>7.2999999999999995E-2</v>
-      </c>
-      <c r="W8" s="7">
-        <v>0.78</v>
-      </c>
-      <c r="X8" s="8">
-        <v>1.54</v>
-      </c>
-      <c r="Y8" s="8">
-        <v>0.69</v>
-      </c>
-      <c r="Z8" s="9">
-        <v>7.3999999999999996E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" s="18" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:26" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C11" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="L11" s="16"/>
-      <c r="M11" s="16"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="P11" s="16"/>
-      <c r="Q11" s="16"/>
-      <c r="R11" s="17"/>
-      <c r="S11" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="T11" s="16"/>
-      <c r="U11" s="16"/>
-      <c r="V11" s="17"/>
-      <c r="W11" s="14"/>
-      <c r="X11" s="14"/>
-      <c r="Y11" s="14"/>
-      <c r="Z11" s="14"/>
-    </row>
-    <row r="12" spans="1:26" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:33" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="D12" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="E12" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="F12" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="G12" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="H12" s="14"/>
+      <c r="I12" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="J12" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="I12" s="10" t="s">
+      <c r="K12" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="J12" s="5" t="s">
+      <c r="L12" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="K12" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="L12" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="M12" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="N12" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="O12" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="P12" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q12" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="R12" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="S12" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="T12" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="U12" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="V12" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="W12" s="10"/>
-      <c r="X12" s="10"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="5"/>
+      <c r="S12" s="4"/>
+      <c r="T12" s="10"/>
+      <c r="U12" s="10"/>
+      <c r="V12" s="5"/>
+      <c r="W12" s="14"/>
+      <c r="X12" s="4"/>
       <c r="Y12" s="10"/>
       <c r="Z12" s="10"/>
+      <c r="AA12" s="5"/>
+      <c r="AB12" s="14"/>
+      <c r="AC12" s="14"/>
+      <c r="AD12" s="10"/>
+      <c r="AE12" s="10"/>
+      <c r="AF12" s="10"/>
+      <c r="AG12" s="10"/>
     </row>
-    <row r="13" spans="1:26" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:33" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
+        <v>0</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0.91</v>
+      </c>
+      <c r="E13" s="10">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="F13" s="10">
+        <v>0.82</v>
+      </c>
+      <c r="G13" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="H13" s="14">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="I13" s="4">
+        <v>0.78</v>
+      </c>
+      <c r="J13" s="10">
+        <v>1.38</v>
+      </c>
+      <c r="K13" s="10">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="L13" s="5">
+        <v>0.184</v>
+      </c>
+      <c r="M13" s="14">
+        <v>0.64</v>
+      </c>
+      <c r="N13" s="4">
+        <v>0.59</v>
+      </c>
+      <c r="O13" s="10">
+        <v>1.05</v>
+      </c>
+      <c r="P13" s="10">
+        <v>0.66</v>
+      </c>
+      <c r="Q13" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="R13" s="26">
+        <v>0.65</v>
+      </c>
+      <c r="S13" s="4">
+        <v>0.81</v>
+      </c>
+      <c r="T13" s="10">
+        <v>1.96</v>
+      </c>
+      <c r="U13" s="10">
+        <v>0.68</v>
+      </c>
+      <c r="V13" s="5">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="W13" s="14">
+        <v>0.66</v>
+      </c>
+      <c r="X13" s="4">
+        <v>0.92</v>
+      </c>
+      <c r="Y13" s="10">
+        <v>1.5</v>
+      </c>
+      <c r="Z13" s="10">
+        <v>0.83</v>
+      </c>
+      <c r="AA13" s="5">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="AB13" s="14"/>
+      <c r="AC13" s="14"/>
+      <c r="AD13" s="10"/>
+      <c r="AE13" s="10"/>
+      <c r="AF13" s="10"/>
+      <c r="AG13" s="10"/>
+    </row>
+    <row r="14" spans="1:33" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>0</v>
+      </c>
+      <c r="B14" s="1">
         <v>1</v>
       </c>
-      <c r="B13" s="1">
+      <c r="C14" s="1">
+        <v>0.71</v>
+      </c>
+      <c r="D14" s="4">
+        <v>0.76</v>
+      </c>
+      <c r="E14" s="10">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="F14" s="10">
+        <v>0.69</v>
+      </c>
+      <c r="G14" s="5">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="H14" s="14">
+        <v>0.46</v>
+      </c>
+      <c r="I14" s="4">
+        <v>0.64</v>
+      </c>
+      <c r="J14" s="10">
+        <v>1.38</v>
+      </c>
+      <c r="K14" s="10">
+        <v>0.48</v>
+      </c>
+      <c r="L14" s="5">
+        <v>0.185</v>
+      </c>
+      <c r="M14" s="14">
+        <v>0.53</v>
+      </c>
+      <c r="N14" s="4">
+        <v>0.48</v>
+      </c>
+      <c r="O14" s="10">
+        <v>1.05</v>
+      </c>
+      <c r="P14" s="10">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="Q14" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="R14" s="26">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="S14" s="4">
+        <v>0.68</v>
+      </c>
+      <c r="T14" s="10">
+        <v>1.96</v>
+      </c>
+      <c r="U14" s="10">
+        <v>0.62</v>
+      </c>
+      <c r="V14" s="5">
+        <v>0.06</v>
+      </c>
+      <c r="W14" s="14">
+        <v>0.61</v>
+      </c>
+      <c r="X14" s="4">
+        <v>0.78</v>
+      </c>
+      <c r="Y14" s="10">
+        <v>1.5</v>
+      </c>
+      <c r="Z14" s="10">
+        <v>0.78</v>
+      </c>
+      <c r="AA14" s="5">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="AB14" s="14"/>
+      <c r="AC14" s="14"/>
+      <c r="AD14" s="10"/>
+      <c r="AE14" s="10"/>
+      <c r="AF14" s="10"/>
+      <c r="AG14" s="10"/>
+    </row>
+    <row r="15" spans="1:33" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
         <v>1</v>
       </c>
-      <c r="C13" s="4">
+      <c r="B15" s="2">
+        <v>0</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.77</v>
+      </c>
+      <c r="D15" s="6">
+        <v>0.82</v>
+      </c>
+      <c r="E15" s="3">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="F15" s="10">
+        <v>0.74</v>
+      </c>
+      <c r="G15" s="5">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="H15" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="I15" s="4">
         <v>0.69</v>
       </c>
-      <c r="D13" s="10">
-        <v>1.1100000000000001</v>
-      </c>
-      <c r="E13" s="10">
-        <v>0.65</v>
-      </c>
-      <c r="F13" s="5">
-        <v>0.252</v>
-      </c>
-      <c r="G13" s="4">
+      <c r="J15" s="10">
+        <v>1.38</v>
+      </c>
+      <c r="K15" s="10">
+        <v>0.51</v>
+      </c>
+      <c r="L15" s="5">
+        <v>0.186</v>
+      </c>
+      <c r="M15" s="14">
+        <v>0.63</v>
+      </c>
+      <c r="N15" s="4">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="O15" s="10">
+        <v>1.05</v>
+      </c>
+      <c r="P15" s="10">
+        <v>0.64</v>
+      </c>
+      <c r="Q15" s="5">
+        <v>0.501</v>
+      </c>
+      <c r="R15" s="26">
         <v>0.59</v>
       </c>
-      <c r="H13" s="10">
-        <v>1.17</v>
-      </c>
-      <c r="I13" s="10">
-        <v>0.54</v>
-      </c>
-      <c r="J13" s="5">
-        <v>0.191</v>
-      </c>
-      <c r="K13" s="4">
-        <v>0.49</v>
-      </c>
-      <c r="L13" s="10">
-        <v>1.1399999999999999</v>
-      </c>
-      <c r="M13" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="N13" s="5">
-        <v>5.0999999999999997E-2</v>
-      </c>
-      <c r="O13" s="4">
+      <c r="S15" s="4">
+        <v>0.69</v>
+      </c>
+      <c r="T15" s="10">
+        <v>1.96</v>
+      </c>
+      <c r="U15" s="10">
         <v>0.62</v>
       </c>
-      <c r="P13" s="10">
-        <v>1.1399999999999999</v>
-      </c>
-      <c r="Q13" s="10">
+      <c r="V15" s="5">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="W15" s="14">
+        <v>0.6</v>
+      </c>
+      <c r="X15" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="Y15" s="10">
+        <v>1.5</v>
+      </c>
+      <c r="Z15" s="10">
+        <v>0.78</v>
+      </c>
+      <c r="AA15" s="5">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="AB15" s="14"/>
+      <c r="AC15" s="14"/>
+      <c r="AD15" s="10"/>
+      <c r="AE15" s="10"/>
+      <c r="AF15" s="10"/>
+      <c r="AG15" s="10"/>
+    </row>
+    <row r="16" spans="1:33" s="8" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="8">
+        <v>1</v>
+      </c>
+      <c r="B16" s="8">
+        <v>1</v>
+      </c>
+      <c r="C16" s="8">
+        <v>0.69</v>
+      </c>
+      <c r="D16" s="7">
+        <v>0.74</v>
+      </c>
+      <c r="E16" s="8">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="F16" s="8">
+        <v>0.67</v>
+      </c>
+      <c r="G16" s="9">
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="H16" s="8">
+        <v>0.44</v>
+      </c>
+      <c r="I16" s="7">
+        <v>0.61</v>
+      </c>
+      <c r="J16" s="8">
+        <v>1.38</v>
+      </c>
+      <c r="K16" s="8">
+        <v>0.46</v>
+      </c>
+      <c r="L16" s="9">
+        <v>0.186</v>
+      </c>
+      <c r="M16" s="8">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="N16" s="7">
+        <v>0.52</v>
+      </c>
+      <c r="O16" s="8">
+        <v>1.05</v>
+      </c>
+      <c r="P16" s="8">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="Q16" s="9">
+        <v>0.501</v>
+      </c>
+      <c r="R16" s="8">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="S16" s="7">
+        <v>0.66</v>
+      </c>
+      <c r="T16" s="8">
+        <v>1.96</v>
+      </c>
+      <c r="U16" s="8">
+        <v>0.6</v>
+      </c>
+      <c r="V16" s="9">
+        <v>6.2E-2</v>
+      </c>
+      <c r="W16" s="8">
+        <v>0.6</v>
+      </c>
+      <c r="X16" s="7">
+        <v>0.76</v>
+      </c>
+      <c r="Y16" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="Z16" s="8">
         <v>0.77</v>
       </c>
-      <c r="R13" s="5">
-        <v>0.06</v>
-      </c>
-      <c r="S13" s="4">
-        <v>0.73</v>
-      </c>
-      <c r="T13" s="10">
-        <v>1.17</v>
-      </c>
-      <c r="U13" s="10">
-        <v>0.84</v>
-      </c>
-      <c r="V13" s="5">
-        <v>8.1000000000000003E-2</v>
-      </c>
-      <c r="W13" s="10"/>
-      <c r="X13" s="10"/>
-      <c r="Y13" s="10"/>
-      <c r="Z13" s="10"/>
+      <c r="AA16" s="9">
+        <v>7.0000000000000007E-2</v>
+      </c>
     </row>
-    <row r="14" spans="1:26" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
-        <v>1</v>
-      </c>
-      <c r="B14" s="1">
-        <v>0</v>
-      </c>
-      <c r="C14" s="4">
-        <v>0.76</v>
-      </c>
-      <c r="D14" s="10">
-        <v>1.1100000000000001</v>
-      </c>
-      <c r="E14" s="10">
-        <v>0.71</v>
-      </c>
-      <c r="F14" s="5">
-        <v>0.25</v>
-      </c>
-      <c r="G14" s="4">
-        <v>0.65</v>
-      </c>
-      <c r="H14" s="10">
-        <v>1.17</v>
-      </c>
-      <c r="I14" s="10">
-        <v>0.59</v>
-      </c>
-      <c r="J14" s="5">
-        <v>0.191</v>
-      </c>
-      <c r="K14" s="4">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="L14" s="10">
-        <v>1.1399999999999999</v>
-      </c>
-      <c r="M14" s="10">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="N14" s="5">
-        <v>5.0999999999999997E-2</v>
-      </c>
-      <c r="O14" s="4">
-        <v>0.68</v>
-      </c>
-      <c r="P14" s="10">
-        <v>1.1399999999999999</v>
-      </c>
-      <c r="Q14" s="10">
-        <v>0.81</v>
-      </c>
-      <c r="R14" s="5">
-        <v>6.0999999999999999E-2</v>
-      </c>
-      <c r="S14" s="4">
-        <v>0.77</v>
-      </c>
-      <c r="T14" s="10">
-        <v>1.17</v>
-      </c>
-      <c r="U14" s="10">
-        <v>0.86</v>
-      </c>
-      <c r="V14" s="5">
-        <v>0.08</v>
-      </c>
-      <c r="W14" s="10"/>
-      <c r="X14" s="10"/>
-      <c r="Y14" s="10"/>
-      <c r="Z14" s="10"/>
+    <row r="17" spans="2:24" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I17" s="12"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="14"/>
+      <c r="S17" s="12"/>
+      <c r="X17" s="12"/>
     </row>
-    <row r="15" spans="1:26" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
-        <v>0</v>
-      </c>
-      <c r="B15" s="2">
-        <v>1</v>
-      </c>
-      <c r="C15" s="6">
-        <v>0.71</v>
-      </c>
-      <c r="D15" s="3">
-        <v>1.1100000000000001</v>
-      </c>
-      <c r="E15" s="10">
-        <v>0.67</v>
-      </c>
-      <c r="F15" s="5">
-        <v>0.251</v>
-      </c>
-      <c r="G15" s="4">
-        <v>0.61</v>
-      </c>
-      <c r="H15" s="10">
-        <v>1.17</v>
-      </c>
-      <c r="I15" s="10">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="J15" s="5">
-        <v>0.19</v>
-      </c>
-      <c r="K15" s="4">
-        <v>0.45</v>
-      </c>
-      <c r="L15" s="10">
-        <v>1.1399999999999999</v>
-      </c>
-      <c r="M15" s="10">
-        <v>0.48</v>
-      </c>
-      <c r="N15" s="5">
-        <v>0.05</v>
-      </c>
-      <c r="O15" s="4">
-        <v>0.64</v>
-      </c>
-      <c r="P15" s="10">
-        <v>1.1399999999999999</v>
-      </c>
-      <c r="Q15" s="10">
-        <v>0.78</v>
-      </c>
-      <c r="R15" s="5">
-        <v>5.8000000000000003E-2</v>
-      </c>
-      <c r="S15" s="4">
-        <v>0.75</v>
-      </c>
-      <c r="T15" s="10">
-        <v>1.17</v>
-      </c>
-      <c r="U15" s="10">
-        <v>0.85</v>
-      </c>
-      <c r="V15" s="5">
-        <v>0.08</v>
-      </c>
-      <c r="W15" s="10"/>
-      <c r="X15" s="10"/>
-      <c r="Y15" s="10"/>
-      <c r="Z15" s="10"/>
-    </row>
-    <row r="16" spans="1:26" s="8" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="8">
-        <v>0</v>
-      </c>
-      <c r="B16" s="8">
-        <v>0</v>
-      </c>
-      <c r="C16" s="7">
-        <v>0.82</v>
-      </c>
-      <c r="D16" s="8">
-        <v>1.1100000000000001</v>
-      </c>
-      <c r="E16" s="8">
-        <v>0.78</v>
-      </c>
-      <c r="F16" s="9">
-        <v>0.248</v>
-      </c>
-      <c r="G16" s="7">
-        <v>0.74</v>
-      </c>
-      <c r="H16" s="8">
-        <v>1.17</v>
-      </c>
-      <c r="I16" s="8">
-        <v>0.67</v>
-      </c>
-      <c r="J16" s="9">
-        <v>0.19</v>
-      </c>
-      <c r="K16" s="7">
-        <v>0.53</v>
-      </c>
-      <c r="L16" s="8">
-        <v>1.1399999999999999</v>
-      </c>
-      <c r="M16" s="8">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="N16" s="9">
-        <v>0.05</v>
-      </c>
-      <c r="O16" s="7">
-        <v>0.73</v>
-      </c>
-      <c r="P16" s="8">
-        <v>1.1399999999999999</v>
-      </c>
-      <c r="Q16" s="8">
-        <v>0.84</v>
-      </c>
-      <c r="R16" s="9">
-        <v>5.7000000000000002E-2</v>
-      </c>
-      <c r="S16" s="7">
-        <v>0.84</v>
-      </c>
-      <c r="T16" s="8">
-        <v>1.17</v>
-      </c>
-      <c r="U16" s="8">
-        <v>0.9</v>
-      </c>
-      <c r="V16" s="9">
-        <v>7.5999999999999998E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="2:19" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G17" s="12"/>
-      <c r="J17" s="13"/>
-      <c r="O17" s="12"/>
-      <c r="S17" s="12"/>
-    </row>
-    <row r="21" spans="2:19" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:24" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="2:19" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C22" s="1" t="s">
+    <row r="22" spans="2:24" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="G22" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="I22" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="J22" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I22" s="1" t="s">
+      <c r="K22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N22" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K22" s="1" t="s">
+      <c r="O22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S22" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L22" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M22" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="O22" s="1" t="s">
+      <c r="T22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="P22" s="1" t="s">
+      <c r="U22" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="Q22" s="1" t="s">
+      <c r="V22" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="R22" s="1" t="s">
-        <v>22</v>
-      </c>
     </row>
-    <row r="23" spans="2:19" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C23" s="12">
-        <v>0.75</v>
-      </c>
-      <c r="D23" s="12">
-        <v>0.74</v>
-      </c>
-      <c r="E23" s="12">
-        <v>0.72</v>
-      </c>
-      <c r="F23" s="12">
-        <v>0.76</v>
-      </c>
-      <c r="G23" s="12">
-        <v>0.71</v>
-      </c>
-      <c r="H23" s="12">
-        <v>0.65</v>
-      </c>
-      <c r="I23" s="12">
-        <v>0.69</v>
-      </c>
-      <c r="J23" s="12">
-        <v>0.59</v>
-      </c>
-      <c r="K23" s="12">
-        <v>0.49</v>
-      </c>
-      <c r="L23" s="12">
-        <v>0.62</v>
-      </c>
-      <c r="M23" s="12">
-        <v>0.73</v>
-      </c>
+    <row r="23" spans="2:24" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="12"/>
+      <c r="O23" s="12"/>
+      <c r="P23" s="12"/>
     </row>
-    <row r="24" spans="2:19" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C24" s="12">
-        <v>0.8</v>
-      </c>
-      <c r="D24" s="12">
-        <v>0.79</v>
-      </c>
-      <c r="E24" s="12">
-        <v>0.77</v>
-      </c>
-      <c r="F24" s="12">
-        <v>0.8</v>
-      </c>
-      <c r="G24" s="12">
-        <v>0.76</v>
-      </c>
-      <c r="H24" s="12">
-        <v>0.7</v>
-      </c>
-      <c r="I24" s="12">
-        <v>0.76</v>
-      </c>
-      <c r="J24" s="12">
-        <v>0.65</v>
-      </c>
-      <c r="K24" s="12">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="L24" s="12">
-        <v>0.68</v>
-      </c>
-      <c r="M24" s="12">
-        <v>0.77</v>
-      </c>
+    <row r="24" spans="2:24" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="12"/>
+      <c r="N24" s="12"/>
+      <c r="O24" s="12"/>
+      <c r="P24" s="12"/>
     </row>
-    <row r="25" spans="2:19" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C25" s="6">
-        <v>0.76</v>
-      </c>
-      <c r="D25" s="12">
-        <v>0.76</v>
-      </c>
-      <c r="E25" s="12">
-        <v>0.74</v>
-      </c>
-      <c r="F25" s="12">
-        <v>0.79</v>
-      </c>
-      <c r="G25" s="12">
-        <v>0.73</v>
-      </c>
-      <c r="H25" s="12">
-        <v>0.67</v>
-      </c>
-      <c r="I25" s="6">
-        <v>0.71</v>
-      </c>
-      <c r="J25" s="12">
-        <v>0.61</v>
-      </c>
-      <c r="K25" s="12">
-        <v>0.45</v>
-      </c>
-      <c r="L25" s="12">
-        <v>0.64</v>
-      </c>
-      <c r="M25" s="12">
-        <v>0.75</v>
-      </c>
+    <row r="25" spans="2:24" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D25" s="6"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="12"/>
+      <c r="N25" s="12"/>
+      <c r="O25" s="12"/>
+      <c r="P25" s="12"/>
     </row>
-    <row r="26" spans="2:19" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C26" s="7">
-        <v>0.88</v>
-      </c>
-      <c r="D26" s="7">
-        <v>0.88</v>
-      </c>
-      <c r="E26" s="7">
-        <v>0.86</v>
-      </c>
-      <c r="F26" s="7">
-        <v>0.91</v>
-      </c>
-      <c r="G26" s="7">
-        <v>0.85</v>
-      </c>
-      <c r="H26" s="7">
-        <v>0.78</v>
-      </c>
-      <c r="I26" s="7">
-        <v>0.82</v>
-      </c>
-      <c r="J26" s="7">
-        <v>0.74</v>
-      </c>
-      <c r="K26" s="7">
-        <v>0.53</v>
-      </c>
-      <c r="L26" s="7">
-        <v>0.73</v>
-      </c>
-      <c r="M26" s="7">
-        <v>0.84</v>
-      </c>
+    <row r="26" spans="2:24" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="7"/>
+      <c r="P26" s="7"/>
     </row>
-    <row r="28" spans="2:19" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:24" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="2:19" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C29" s="11">
-        <v>0.65</v>
-      </c>
-      <c r="D29" s="11">
-        <v>0.64</v>
-      </c>
-      <c r="E29" s="11">
-        <v>0.7</v>
-      </c>
-      <c r="F29" s="11">
-        <v>0.73</v>
-      </c>
-      <c r="G29" s="11">
-        <v>0.63</v>
-      </c>
-      <c r="H29" s="11">
-        <v>0.61</v>
-      </c>
-      <c r="I29" s="11">
-        <v>0.65</v>
-      </c>
-      <c r="J29" s="11">
-        <v>0.54</v>
-      </c>
-      <c r="K29" s="11">
-        <v>0.5</v>
-      </c>
-      <c r="L29" s="11">
-        <v>0.77</v>
-      </c>
-      <c r="M29" s="11">
-        <v>0.84</v>
-      </c>
+    <row r="29" spans="2:24" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="11"/>
+      <c r="M29" s="14"/>
+      <c r="N29" s="11"/>
+      <c r="O29" s="11"/>
+      <c r="P29" s="11"/>
     </row>
-    <row r="30" spans="2:19" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C30" s="11">
-        <v>0.68</v>
-      </c>
-      <c r="D30" s="11">
-        <v>0.67</v>
-      </c>
-      <c r="E30" s="11">
-        <v>0.73</v>
-      </c>
-      <c r="F30" s="11">
-        <v>0.75</v>
-      </c>
-      <c r="G30" s="11">
-        <v>0.66</v>
-      </c>
-      <c r="H30" s="11">
-        <v>0.63</v>
-      </c>
-      <c r="I30" s="11">
-        <v>0.71</v>
-      </c>
-      <c r="J30" s="11">
-        <v>0.59</v>
-      </c>
-      <c r="K30" s="11">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="L30" s="11">
-        <v>0.81</v>
-      </c>
-      <c r="M30" s="11">
-        <v>0.86</v>
-      </c>
+    <row r="30" spans="2:24" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="11"/>
+      <c r="M30" s="14"/>
+      <c r="N30" s="11"/>
+      <c r="O30" s="11"/>
+      <c r="P30" s="11"/>
     </row>
-    <row r="31" spans="2:19" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C31" s="11">
-        <v>0.66</v>
-      </c>
-      <c r="D31" s="11">
-        <v>0.65</v>
-      </c>
-      <c r="E31" s="11">
-        <v>0.71</v>
-      </c>
-      <c r="F31" s="11">
-        <v>0.75</v>
-      </c>
-      <c r="G31" s="11">
-        <v>0.65</v>
-      </c>
-      <c r="H31" s="11">
-        <v>0.62</v>
-      </c>
-      <c r="I31" s="11">
-        <v>0.67</v>
-      </c>
-      <c r="J31" s="11">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="K31" s="11">
-        <v>0.48</v>
-      </c>
-      <c r="L31" s="11">
-        <v>0.78</v>
-      </c>
-      <c r="M31" s="11">
-        <v>0.85</v>
-      </c>
+    <row r="31" spans="2:24" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="11"/>
+      <c r="L31" s="11"/>
+      <c r="M31" s="14"/>
+      <c r="N31" s="11"/>
+      <c r="O31" s="11"/>
+      <c r="P31" s="11"/>
     </row>
-    <row r="32" spans="2:19" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C32" s="8">
-        <v>0.73</v>
-      </c>
-      <c r="D32" s="8">
-        <v>0.72</v>
-      </c>
-      <c r="E32" s="8">
-        <v>0.78</v>
-      </c>
-      <c r="F32" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="G32" s="8">
-        <v>0.71</v>
-      </c>
-      <c r="H32" s="8">
-        <v>0.69</v>
-      </c>
-      <c r="I32" s="8">
-        <v>0.78</v>
-      </c>
-      <c r="J32" s="8">
-        <v>0.67</v>
-      </c>
-      <c r="K32" s="8">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="L32" s="8">
-        <v>0.84</v>
-      </c>
-      <c r="M32" s="8">
-        <v>0.9</v>
-      </c>
+    <row r="32" spans="2:24" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="8"/>
+      <c r="K32" s="8"/>
+      <c r="L32" s="8"/>
+      <c r="M32" s="8"/>
+      <c r="N32" s="8"/>
+      <c r="O32" s="8"/>
+      <c r="P32" s="8"/>
     </row>
-    <row r="34" spans="2:13" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:16" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="35" spans="2:13" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C35" s="11">
-        <v>0.113</v>
-      </c>
-      <c r="D35" s="13">
-        <v>6.2E-2</v>
-      </c>
-      <c r="E35" s="13">
-        <v>6.4000000000000001E-2</v>
-      </c>
-      <c r="F35" s="13">
-        <v>0.109</v>
-      </c>
-      <c r="G35" s="13">
-        <v>7.5999999999999998E-2</v>
-      </c>
-      <c r="H35" s="13">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="I35" s="13">
-        <v>0.252</v>
-      </c>
-      <c r="J35" s="13">
-        <v>0.191</v>
-      </c>
-      <c r="K35" s="13">
-        <v>5.0999999999999997E-2</v>
-      </c>
-      <c r="L35" s="13">
-        <v>0.06</v>
-      </c>
-      <c r="M35" s="13">
-        <v>8.1000000000000003E-2</v>
-      </c>
+    <row r="35" spans="2:16" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D35" s="11"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="13"/>
+      <c r="K35" s="13"/>
+      <c r="L35" s="13"/>
+      <c r="M35" s="13"/>
+      <c r="N35" s="13"/>
+      <c r="O35" s="13"/>
+      <c r="P35" s="13"/>
     </row>
-    <row r="36" spans="2:13" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C36" s="11">
-        <v>0.113</v>
-      </c>
-      <c r="D36" s="13">
-        <v>6.0999999999999999E-2</v>
-      </c>
-      <c r="E36" s="13">
-        <v>6.4000000000000001E-2</v>
-      </c>
-      <c r="F36" s="13">
-        <v>0.107</v>
-      </c>
-      <c r="G36" s="13">
-        <v>7.5999999999999998E-2</v>
-      </c>
-      <c r="H36" s="13">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="I36" s="13">
-        <v>0.25</v>
-      </c>
-      <c r="J36" s="13">
-        <v>0.191</v>
-      </c>
-      <c r="K36" s="13">
-        <v>5.0999999999999997E-2</v>
-      </c>
-      <c r="L36" s="13">
-        <v>6.0999999999999999E-2</v>
-      </c>
-      <c r="M36" s="13">
-        <v>0.08</v>
-      </c>
+    <row r="36" spans="2:16" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D36" s="11"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="13"/>
+      <c r="K36" s="13"/>
+      <c r="L36" s="13"/>
+      <c r="M36" s="13"/>
+      <c r="N36" s="13"/>
+      <c r="O36" s="13"/>
+      <c r="P36" s="13"/>
     </row>
-    <row r="37" spans="2:13" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C37" s="11">
-        <v>0.111</v>
-      </c>
-      <c r="D37" s="13">
-        <v>6.0999999999999999E-2</v>
-      </c>
-      <c r="E37" s="13">
-        <v>6.4000000000000001E-2</v>
-      </c>
-      <c r="F37" s="13">
-        <v>0.107</v>
-      </c>
-      <c r="G37" s="13">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="H37" s="13">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="I37" s="13">
-        <v>0.251</v>
-      </c>
-      <c r="J37" s="13">
-        <v>0.19</v>
-      </c>
-      <c r="K37" s="13">
-        <v>0.05</v>
-      </c>
-      <c r="L37" s="13">
-        <v>5.8000000000000003E-2</v>
-      </c>
-      <c r="M37" s="13">
-        <v>0.08</v>
-      </c>
+    <row r="37" spans="2:16" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D37" s="11"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="13"/>
+      <c r="K37" s="13"/>
+      <c r="L37" s="13"/>
+      <c r="M37" s="13"/>
+      <c r="N37" s="13"/>
+      <c r="O37" s="13"/>
+      <c r="P37" s="13"/>
     </row>
-    <row r="38" spans="2:13" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C38" s="9">
-        <v>0.11</v>
-      </c>
-      <c r="D38" s="9">
-        <v>5.8999999999999997E-2</v>
-      </c>
-      <c r="E38" s="9">
-        <v>6.2E-2</v>
-      </c>
-      <c r="F38" s="9">
-        <v>0.10299999999999999</v>
-      </c>
-      <c r="G38" s="9">
-        <v>7.2999999999999995E-2</v>
-      </c>
-      <c r="H38" s="9">
-        <v>7.3999999999999996E-2</v>
-      </c>
-      <c r="I38" s="9">
-        <v>0.248</v>
-      </c>
-      <c r="J38" s="9">
-        <v>0.19</v>
-      </c>
-      <c r="K38" s="9">
-        <v>0.05</v>
-      </c>
-      <c r="L38" s="9">
-        <v>5.7000000000000002E-2</v>
-      </c>
-      <c r="M38" s="9">
-        <v>7.5999999999999998E-2</v>
-      </c>
+    <row r="38" spans="2:16" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="9"/>
+      <c r="J38" s="9"/>
+      <c r="K38" s="9"/>
+      <c r="L38" s="9"/>
+      <c r="M38" s="9"/>
+      <c r="N38" s="9"/>
+      <c r="O38" s="9"/>
+      <c r="P38" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="G3:J3"/>
-    <mergeCell ref="K3:N3"/>
-    <mergeCell ref="O3:R3"/>
+    <mergeCell ref="AD3:AG3"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="I11:L11"/>
+    <mergeCell ref="N11:Q11"/>
+    <mergeCell ref="S11:V11"/>
+    <mergeCell ref="X11:AA11"/>
+    <mergeCell ref="AD11:AG11"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="I3:L3"/>
+    <mergeCell ref="N3:Q3"/>
     <mergeCell ref="S3:V3"/>
-    <mergeCell ref="W3:Z3"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="G11:J11"/>
-    <mergeCell ref="K11:N11"/>
-    <mergeCell ref="O11:R11"/>
-    <mergeCell ref="S11:V11"/>
-    <mergeCell ref="W11:Z11"/>
+    <mergeCell ref="X3:AA3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>